<commit_message>
repera for load from base and use period, the problem is with stafflist for a specific month
</commit_message>
<xml_diff>
--- a/src/main/resources/upload-dir/department_2024_10.xlsx
+++ b/src/main/resources/upload-dir/department_2024_10.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Поточна робота\Премії\премія_вересень\дані для загрузки\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Поточна робота\Премії\премія файли\премія_листопад\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8113EA8E-D73A-4718-BE8C-93EB0E79CDFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0131EFB-31E7-4B7E-A2A6-ACA738AA2346}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2430" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Відділення" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Відділення!$A$1:$E$116</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="259">
   <si>
     <t>departmentEleksId</t>
   </si>
@@ -805,6 +808,9 @@
   </si>
   <si>
     <t>0137</t>
+  </si>
+  <si>
+    <t>Перинатальний центр</t>
   </si>
 </sst>
 </file>
@@ -833,7 +839,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -841,11 +847,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -857,11 +878,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1075,7 +1105,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1115,7 @@
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="25" width="8.7109375" customWidth="1"/>
+    <col min="6" max="20" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1107,237 +1137,237 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>143</v>
+        <v>97</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>144</v>
+        <v>242</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>125</v>
+      </c>
+      <c r="E3" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>53</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>17</v>
+        <v>49</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="E9" s="3">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>151</v>
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="3">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>10</v>
+        <v>59</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>8</v>
@@ -1345,16 +1375,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -1362,220 +1392,220 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="E17" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>32</v>
+        <v>46</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>161</v>
+        <v>226</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>34</v>
+        <v>108</v>
+      </c>
+      <c r="E20" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>162</v>
+        <v>222</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="3">
-        <v>55</v>
+        <v>9</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>165</v>
+        <v>257</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>42</v>
+        <v>141</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E25" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>167</v>
+        <v>227</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>10</v>
+        <v>109</v>
+      </c>
+      <c r="E26" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
+        <v>28</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0</v>
+      <c r="E27" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>85</v>
+        <v>991</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>170</v>
+        <v>251</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
@@ -1583,16 +1613,16 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>87</v>
+        <v>992</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>171</v>
+        <v>252</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>47</v>
+        <v>136</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>47</v>
+        <v>136</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
@@ -1600,16 +1630,16 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>89</v>
+        <v>995</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>172</v>
+        <v>254</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
@@ -1617,16 +1647,16 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>90</v>
+        <v>990</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>173</v>
+        <v>250</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
@@ -1634,16 +1664,16 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>174</v>
+        <v>249</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
@@ -1651,16 +1681,16 @@
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
@@ -1668,67 +1698,67 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="3">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>179</v>
+        <v>234</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="E38" s="3">
         <v>9</v>
@@ -1736,33 +1766,33 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="3">
-        <v>9</v>
+        <v>122</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
@@ -1773,33 +1803,33 @@
         <v>32</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>182</v>
+        <v>235</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="E41" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>183</v>
+        <v>239</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="E42" s="3">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1807,16 +1837,16 @@
         <v>32</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>184</v>
+        <v>245</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>42</v>
+        <v>128</v>
+      </c>
+      <c r="E43" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1824,50 +1854,50 @@
         <v>32</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>185</v>
+        <v>248</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0</v>
+        <v>131</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="E45" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="E46" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1875,33 +1905,33 @@
         <v>32</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47" s="3">
-        <v>9</v>
+        <v>117</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1909,13 +1939,13 @@
         <v>32</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E49" s="3">
         <v>0</v>
@@ -1926,64 +1956,64 @@
         <v>32</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>191</v>
+        <v>238</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>42</v>
+        <v>120</v>
+      </c>
+      <c r="E50" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E51" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>193</v>
+        <v>243</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="E52" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
@@ -1991,53 +2021,53 @@
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E54" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="E55" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>197</v>
+        <v>149</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E56" s="3">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2045,13 +2075,13 @@
         <v>32</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E57" s="3">
         <v>9</v>
@@ -2059,16 +2089,16 @@
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>199</v>
+        <v>157</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="E58" s="3">
         <v>0</v>
@@ -2076,33 +2106,33 @@
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>82</v>
+        <v>112</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E60" s="3">
         <v>0</v>
@@ -2113,13 +2143,13 @@
         <v>32</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="E61" s="3">
         <v>9</v>
@@ -2127,70 +2157,70 @@
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>32</v>
+        <v>993</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>203</v>
+        <v>253</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="E62" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E63" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E64" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>206</v>
+        <v>155</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E65" s="3">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2198,13 +2228,13 @@
         <v>32</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>42</v>
@@ -2212,19 +2242,19 @@
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>90</v>
+        <v>80</v>
+      </c>
+      <c r="E67" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2232,13 +2262,13 @@
         <v>81</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E68" s="3">
         <v>0</v>
@@ -2246,118 +2276,118 @@
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E69" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E70" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="E71" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="E72" s="3">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>214</v>
+        <v>168</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="E73" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="E74" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>-1</v>
+        <v>81</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E75" s="3">
         <v>0</v>
@@ -2365,16 +2395,16 @@
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E76" s="3">
         <v>0</v>
@@ -2382,50 +2412,50 @@
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="E77" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E78" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="E79" s="3">
         <v>0</v>
@@ -2436,13 +2466,13 @@
         <v>81</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E80" s="3">
         <v>0</v>
@@ -2450,36 +2480,36 @@
     </row>
     <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>105</v>
+        <v>114</v>
+      </c>
+      <c r="E81" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E82" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2487,30 +2517,30 @@
         <v>32</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E83" s="3">
-        <v>9</v>
+        <v>88</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E84" s="3">
         <v>0</v>
@@ -2518,50 +2548,50 @@
     </row>
     <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>226</v>
+        <v>163</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="E85" s="3">
-        <v>9</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E86" s="3">
-        <v>9</v>
+        <v>54</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E87" s="3">
         <v>0</v>
@@ -2569,16 +2599,16 @@
     </row>
     <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>229</v>
+        <v>172</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>111</v>
+        <v>48</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="E88" s="3">
         <v>0</v>
@@ -2586,16 +2616,16 @@
     </row>
     <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>32</v>
+        <v>-1</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E89" s="3">
         <v>0</v>
@@ -2603,50 +2633,50 @@
     </row>
     <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>231</v>
+        <v>160</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E90" s="3">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>232</v>
+        <v>151</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="E91" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="E92" s="3">
         <v>0</v>
@@ -2654,19 +2684,19 @@
     </row>
     <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>234</v>
+        <v>150</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E93" s="3">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="E93" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2674,13 +2704,13 @@
         <v>32</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="E94" s="3">
         <v>9</v>
@@ -2688,36 +2718,36 @@
     </row>
     <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>236</v>
+        <v>164</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E96" s="3">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2725,13 +2755,13 @@
         <v>32</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>238</v>
+        <v>211</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="E97" s="3">
         <v>9</v>
@@ -2739,16 +2769,16 @@
     </row>
     <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>239</v>
+        <v>180</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>121</v>
+        <v>57</v>
       </c>
       <c r="E98" s="3">
         <v>9</v>
@@ -2759,30 +2789,30 @@
         <v>32</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>240</v>
+        <v>193</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E99" s="4" t="s">
-        <v>123</v>
+        <v>73</v>
+      </c>
+      <c r="E99" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="E100" s="3">
         <v>0</v>
@@ -2793,30 +2823,30 @@
         <v>32</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>242</v>
+        <v>185</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="E101" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>243</v>
+        <v>196</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="E102" s="3">
         <v>0</v>
@@ -2824,19 +2854,19 @@
     </row>
     <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>244</v>
+        <v>165</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E103" s="3">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2844,16 +2874,16 @@
         <v>32</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="E104" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2861,81 +2891,81 @@
         <v>32</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E105" s="4" t="s">
-        <v>42</v>
+        <v>110</v>
+      </c>
+      <c r="E105" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>247</v>
+        <v>183</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
       <c r="E106" s="3">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>248</v>
+        <v>148</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>131</v>
+        <v>16</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="E108" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>990</v>
+        <v>81</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="E109" s="3">
         <v>0</v>
@@ -2943,84 +2973,84 @@
     </row>
     <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>991</v>
+        <v>32</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>135</v>
+        <v>31</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E110" s="3">
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>992</v>
+        <v>32</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>252</v>
+        <v>210</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="E111" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>993</v>
+        <v>18</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>253</v>
+        <v>152</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>137</v>
+        <v>22</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E112" s="3">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>995</v>
+        <v>32</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>254</v>
+        <v>191</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E113" s="3">
-        <v>0</v>
+        <v>71</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E114" s="3">
         <v>0</v>
@@ -3028,16 +3058,16 @@
     </row>
     <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E115" s="3">
         <v>0</v>
@@ -3045,16 +3075,16 @@
     </row>
     <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>257</v>
+        <v>171</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>141</v>
+        <v>47</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>141</v>
+        <v>47</v>
       </c>
       <c r="E116" s="3">
         <v>0</v>
@@ -3945,7 +3975,12 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <autoFilter ref="A1:E116" xr:uid="{274E9404-ED2F-4BF9-BEF8-E87F79CC3CCD}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E116">
+      <sortCondition ref="D1:D116"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>